<commit_message>
sephora search page crawler and also some additions to mapping files
</commit_message>
<xml_diff>
--- a/product_scraper/product_scraper/reference_data/profit_margin_mapping.xlsx
+++ b/product_scraper/product_scraper/reference_data/profit_margin_mapping.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sujilmaharjan/Desktop/qarece-web-crawler/product_scraper/product_scraper/reference_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/CodeForLyf/qarece-web-crawler/product_scraper/product_scraper/reference_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E17CED1-B6D3-7643-ACF4-8F9251E77ABF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F62D9A01-9ABB-D14F-BBF3-492B82139A41}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{DABBC373-DD1C-BE4F-B648-BD9F3D1B3B72}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="190">
   <si>
     <t>Handbags</t>
   </si>
@@ -162,9 +162,6 @@
     <t>Oil &amp; Shine Control</t>
   </si>
   <si>
-    <t>Palette</t>
-  </si>
-  <si>
     <t>Powder</t>
   </si>
   <si>
@@ -598,6 +595,12 @@
   </si>
   <si>
     <t>Self Tanners</t>
+  </si>
+  <si>
+    <t>Nail</t>
+  </si>
+  <si>
+    <t>Fragrances &amp; Perfumes</t>
   </si>
 </sst>
 </file>
@@ -705,10 +708,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{013CB231-6A17-0C41-B34E-8545193EC78F}" name="Table3" displayName="Table3" ref="A1:E197" totalsRowShown="0">
-  <autoFilter ref="A1:E197" xr:uid="{80DC04BB-911F-774F-8154-5B368973EF57}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E197">
-    <sortCondition ref="A1:A1048570"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{013CB231-6A17-0C41-B34E-8545193EC78F}" name="Table3" displayName="Table3" ref="A1:E200" totalsRowShown="0">
+  <autoFilter ref="A1:E200" xr:uid="{80DC04BB-911F-774F-8154-5B368973EF57}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E198">
+    <sortCondition ref="A1:A1048571"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{83132A01-FD6A-FB47-B069-4E276A9F62CE}" name="q_category"/>
@@ -1018,10 +1021,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{674E1AF3-8D38-BC46-B033-52B0C55ED4E6}">
-  <dimension ref="A1:E197"/>
+  <dimension ref="A1:E199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="133" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1033,19 +1036,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" t="s">
         <v>132</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>133</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>134</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>135</v>
-      </c>
-      <c r="E1" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1382,7 +1385,7 @@
         <v>33</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -1399,7 +1402,7 @@
         <v>33</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E22">
         <v>0.5</v>
@@ -1416,7 +1419,7 @@
         <v>33</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E23">
         <v>0.25</v>
@@ -1433,7 +1436,7 @@
         <v>33</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E24">
         <v>0.5</v>
@@ -1450,7 +1453,7 @@
         <v>33</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E25">
         <v>0.5</v>
@@ -1464,10 +1467,10 @@
         <v>22</v>
       </c>
       <c r="C26" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="E26">
         <v>0.2</v>
@@ -1481,10 +1484,10 @@
         <v>22</v>
       </c>
       <c r="C27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E27">
         <v>0.2</v>
@@ -1498,10 +1501,10 @@
         <v>22</v>
       </c>
       <c r="C28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E28">
         <v>0.2</v>
@@ -1515,10 +1518,10 @@
         <v>22</v>
       </c>
       <c r="C29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E29">
         <v>0.2</v>
@@ -1532,10 +1535,10 @@
         <v>22</v>
       </c>
       <c r="C30" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E30">
         <v>1</v>
@@ -1549,10 +1552,10 @@
         <v>22</v>
       </c>
       <c r="C31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E31">
         <v>0.2</v>
@@ -1566,10 +1569,10 @@
         <v>22</v>
       </c>
       <c r="C32" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E32">
         <v>0.2</v>
@@ -1583,10 +1586,10 @@
         <v>22</v>
       </c>
       <c r="C33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E33">
         <v>0.2</v>
@@ -1597,14 +1600,14 @@
         <v>21</v>
       </c>
       <c r="B34" t="s">
-        <v>57</v>
+        <v>22</v>
       </c>
       <c r="C34" t="s">
-        <v>58</v>
+        <v>188</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -1612,14 +1615,14 @@
         <v>21</v>
       </c>
       <c r="B35" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35" t="s">
         <v>57</v>
-      </c>
-      <c r="C35" t="s">
-        <v>59</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -1627,14 +1630,14 @@
         <v>21</v>
       </c>
       <c r="B36" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C36" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -1642,14 +1645,14 @@
         <v>21</v>
       </c>
       <c r="B37" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C37" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -1657,10 +1660,10 @@
         <v>21</v>
       </c>
       <c r="B38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C38" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38">
@@ -1672,10 +1675,10 @@
         <v>21</v>
       </c>
       <c r="B39" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C39" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39">
@@ -1687,14 +1690,14 @@
         <v>21</v>
       </c>
       <c r="B40" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C40" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -1702,16 +1705,14 @@
         <v>21</v>
       </c>
       <c r="B41" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="C41" t="s">
-        <v>48</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>112</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="D41" s="2"/>
       <c r="E41">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -1722,10 +1723,10 @@
         <v>22</v>
       </c>
       <c r="C42" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E42">
         <v>1.5</v>
@@ -1739,13 +1740,13 @@
         <v>22</v>
       </c>
       <c r="C43" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E43">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
@@ -1756,10 +1757,10 @@
         <v>22</v>
       </c>
       <c r="C44" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E44">
         <v>0.5</v>
@@ -1776,10 +1777,10 @@
         <v>33</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E45">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
@@ -1793,7 +1794,7 @@
         <v>33</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E46">
         <v>0.25</v>
@@ -1810,10 +1811,10 @@
         <v>33</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E47">
-        <v>1.5</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
@@ -1823,13 +1824,13 @@
       <c r="B48" t="s">
         <v>22</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>23</v>
+      <c r="C48" t="s">
+        <v>33</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="E48" s="1">
+        <v>117</v>
+      </c>
+      <c r="E48">
         <v>1.5</v>
       </c>
     </row>
@@ -1840,14 +1841,14 @@
       <c r="B49" t="s">
         <v>22</v>
       </c>
-      <c r="C49" t="s">
-        <v>66</v>
+      <c r="C49" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E49">
-        <v>0.25</v>
+        <v>118</v>
+      </c>
+      <c r="E49" s="1">
+        <v>1.5</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
@@ -1858,13 +1859,13 @@
         <v>22</v>
       </c>
       <c r="C50" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E50">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
@@ -1875,13 +1876,13 @@
         <v>22</v>
       </c>
       <c r="C51" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>41</v>
+        <v>120</v>
       </c>
       <c r="E51">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
@@ -1892,13 +1893,13 @@
         <v>22</v>
       </c>
       <c r="C52" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>122</v>
+        <v>41</v>
       </c>
       <c r="E52">
-        <v>0.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
@@ -1909,13 +1910,13 @@
         <v>22</v>
       </c>
       <c r="C53" t="s">
-        <v>23</v>
+        <v>65</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="E53">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
@@ -1926,10 +1927,10 @@
         <v>22</v>
       </c>
       <c r="C54" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E54">
         <v>0.5</v>
@@ -1943,11 +1944,13 @@
         <v>22</v>
       </c>
       <c r="C55" t="s">
-        <v>123</v>
-      </c>
-      <c r="D55" s="2"/>
+        <v>47</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>114</v>
+      </c>
       <c r="E55">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
@@ -1958,11 +1961,11 @@
         <v>22</v>
       </c>
       <c r="C56" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56">
-        <v>1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
@@ -1973,7 +1976,7 @@
         <v>22</v>
       </c>
       <c r="C57" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57">
@@ -1985,14 +1988,14 @@
         <v>21</v>
       </c>
       <c r="B58" t="s">
-        <v>57</v>
+        <v>22</v>
       </c>
       <c r="C58" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58">
-        <v>0.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
@@ -2000,14 +2003,14 @@
         <v>21</v>
       </c>
       <c r="B59" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C59" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D59" s="2"/>
       <c r="E59">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
@@ -2015,10 +2018,10 @@
         <v>21</v>
       </c>
       <c r="B60" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C60" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60">
@@ -2030,12 +2033,12 @@
         <v>21</v>
       </c>
       <c r="B61" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C61" t="s">
-        <v>129</v>
-      </c>
-      <c r="D61" s="1"/>
+        <v>127</v>
+      </c>
+      <c r="D61" s="2"/>
       <c r="E61">
         <v>0.5</v>
       </c>
@@ -2045,13 +2048,14 @@
         <v>21</v>
       </c>
       <c r="B62" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C62" t="s">
-        <v>130</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="D62" s="1"/>
       <c r="E62">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
@@ -2059,98 +2063,101 @@
         <v>21</v>
       </c>
       <c r="B63" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C63" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E63">
         <v>0.25</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A64" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C64" s="5" t="s">
+      <c r="A64" t="s">
+        <v>21</v>
+      </c>
+      <c r="B64" t="s">
+        <v>56</v>
+      </c>
+      <c r="C64" t="s">
+        <v>130</v>
+      </c>
+      <c r="E64">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="D65" s="5"/>
+      <c r="E65">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D66" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="D64" s="5"/>
-      <c r="E64">
+      <c r="E66">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C67" s="5"/>
+      <c r="D67" s="5"/>
+      <c r="E67">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D68" s="6"/>
+      <c r="E68">
         <v>1.5</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A65" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B65" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C65" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="D65" s="6" t="s">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D69" s="5" t="s">
         <v>187</v>
-      </c>
-      <c r="E65">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A66" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C66" s="5"/>
-      <c r="D66" s="5"/>
-      <c r="E66">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A67" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B67" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C67" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="D67" s="6"/>
-      <c r="E67">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A68" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B68" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C68" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D68" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="E68">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>153</v>
-      </c>
-      <c r="B69" t="s">
-        <v>154</v>
       </c>
       <c r="E69">
         <v>1</v>
@@ -2158,13 +2165,13 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>0</v>
+        <v>152</v>
       </c>
       <c r="B70" t="s">
-        <v>12</v>
+        <v>153</v>
       </c>
       <c r="E70">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
@@ -2172,11 +2179,10 @@
         <v>0</v>
       </c>
       <c r="B71" t="s">
-        <v>1</v>
-      </c>
-      <c r="D71" s="1"/>
+        <v>12</v>
+      </c>
       <c r="E71">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
@@ -2184,10 +2190,11 @@
         <v>0</v>
       </c>
       <c r="B72" t="s">
-        <v>2</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D72" s="1"/>
       <c r="E72">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
@@ -2195,10 +2202,10 @@
         <v>0</v>
       </c>
       <c r="B73" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="E73">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
@@ -2206,10 +2213,10 @@
         <v>0</v>
       </c>
       <c r="B74" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E74">
-        <v>2.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
@@ -2217,10 +2224,10 @@
         <v>0</v>
       </c>
       <c r="B75" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="E75">
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
@@ -2228,10 +2235,10 @@
         <v>0</v>
       </c>
       <c r="B76" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="E76">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
@@ -2239,11 +2246,10 @@
         <v>0</v>
       </c>
       <c r="B77" t="s">
-        <v>16</v>
-      </c>
-      <c r="D77" s="1"/>
+        <v>15</v>
+      </c>
       <c r="E77">
-        <v>2.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
@@ -2251,10 +2257,11 @@
         <v>0</v>
       </c>
       <c r="B78" t="s">
-        <v>17</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="D78" s="1"/>
       <c r="E78">
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
@@ -2262,9 +2269,8 @@
         <v>0</v>
       </c>
       <c r="B79" t="s">
-        <v>4</v>
-      </c>
-      <c r="D79" s="1"/>
+        <v>17</v>
+      </c>
       <c r="E79">
         <v>1.5</v>
       </c>
@@ -2274,11 +2280,11 @@
         <v>0</v>
       </c>
       <c r="B80" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D80" s="1"/>
       <c r="E80">
-        <v>3</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
@@ -2286,11 +2292,11 @@
         <v>0</v>
       </c>
       <c r="B81" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D81" s="1"/>
       <c r="E81">
-        <v>2.7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
@@ -2298,10 +2304,11 @@
         <v>0</v>
       </c>
       <c r="B82" t="s">
-        <v>7</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D82" s="1"/>
       <c r="E82">
-        <v>2.5</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
@@ -2309,10 +2316,10 @@
         <v>0</v>
       </c>
       <c r="B83" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="E83">
-        <v>2</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
@@ -2320,10 +2327,10 @@
         <v>0</v>
       </c>
       <c r="B84" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E84">
-        <v>0.8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
@@ -2331,10 +2338,10 @@
         <v>0</v>
       </c>
       <c r="B85" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="E85">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
@@ -2342,7 +2349,7 @@
         <v>0</v>
       </c>
       <c r="B86" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E86">
         <v>0.5</v>
@@ -2353,10 +2360,10 @@
         <v>0</v>
       </c>
       <c r="B87" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E87">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
@@ -2364,10 +2371,10 @@
         <v>0</v>
       </c>
       <c r="B88" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E88">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
@@ -2375,32 +2382,29 @@
         <v>0</v>
       </c>
       <c r="B89" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E89">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>0</v>
       </c>
+      <c r="B90" t="s">
+        <v>20</v>
+      </c>
       <c r="E90">
-        <v>2</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>0</v>
       </c>
-      <c r="B91" t="s">
-        <v>142</v>
-      </c>
-      <c r="C91" t="s">
-        <v>143</v>
-      </c>
       <c r="E91">
-        <v>1.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
@@ -2408,13 +2412,13 @@
         <v>0</v>
       </c>
       <c r="B92" t="s">
+        <v>141</v>
+      </c>
+      <c r="C92" t="s">
         <v>142</v>
       </c>
-      <c r="C92" t="s">
-        <v>146</v>
-      </c>
       <c r="E92">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
@@ -2422,10 +2426,10 @@
         <v>0</v>
       </c>
       <c r="B93" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C93" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E93">
         <v>2</v>
@@ -2436,7 +2440,10 @@
         <v>0</v>
       </c>
       <c r="B94" t="s">
-        <v>149</v>
+        <v>146</v>
+      </c>
+      <c r="C94" t="s">
+        <v>147</v>
       </c>
       <c r="E94">
         <v>2</v>
@@ -2444,10 +2451,10 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>144</v>
+        <v>0</v>
       </c>
       <c r="B95" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="E95">
         <v>2</v>
@@ -2455,6 +2462,9 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
+        <v>143</v>
+      </c>
+      <c r="B96" t="s">
         <v>144</v>
       </c>
       <c r="E96">
@@ -2463,54 +2473,51 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>150</v>
-      </c>
-      <c r="B97" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="E97">
-        <v>1.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
+        <v>149</v>
+      </c>
+      <c r="B98" t="s">
         <v>150</v>
       </c>
-      <c r="B98" t="s">
-        <v>155</v>
-      </c>
       <c r="E98">
-        <v>3</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B99" t="s">
-        <v>90</v>
+        <v>154</v>
       </c>
       <c r="E99">
-        <v>1.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B100" t="s">
-        <v>156</v>
+        <v>89</v>
       </c>
       <c r="E100">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B101" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E101">
         <v>1</v>
@@ -2518,10 +2525,10 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B102" t="s">
-        <v>80</v>
+        <v>156</v>
       </c>
       <c r="E102">
         <v>1</v>
@@ -2529,10 +2536,10 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B103" t="s">
-        <v>158</v>
+        <v>79</v>
       </c>
       <c r="E103">
         <v>1</v>
@@ -2540,98 +2547,98 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B104" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E104">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B105" t="s">
-        <v>87</v>
+        <v>158</v>
       </c>
       <c r="E105">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B106" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="E106">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B107" t="s">
-        <v>160</v>
+        <v>73</v>
       </c>
       <c r="E107">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B108" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E108">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B109" t="s">
-        <v>184</v>
+        <v>160</v>
       </c>
       <c r="E109">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B110" t="s">
-        <v>162</v>
+        <v>183</v>
       </c>
       <c r="E110">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B111" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E111">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B112" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E112">
         <v>1</v>
@@ -2639,51 +2646,51 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B113" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E113">
-        <v>3.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B114" t="s">
-        <v>185</v>
+        <v>164</v>
       </c>
       <c r="E114">
-        <v>1.5</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>150</v>
+        <v>149</v>
+      </c>
+      <c r="B115" t="s">
+        <v>184</v>
       </c>
       <c r="E115">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>150</v>
-      </c>
-      <c r="B116" t="s">
-        <v>96</v>
+        <v>149</v>
       </c>
       <c r="E116">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B117" t="s">
-        <v>166</v>
+        <v>95</v>
       </c>
       <c r="E117">
         <v>1</v>
@@ -2691,33 +2698,33 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B118" t="s">
-        <v>84</v>
-      </c>
-      <c r="D118" s="2"/>
+        <v>165</v>
+      </c>
       <c r="E118">
         <v>1</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B119" t="s">
-        <v>167</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="D119" s="2"/>
       <c r="E119">
         <v>1</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B120" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E120">
         <v>1</v>
@@ -2725,10 +2732,10 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B121" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E121">
         <v>1</v>
@@ -2736,10 +2743,10 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B122" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E122">
         <v>1</v>
@@ -2747,10 +2754,10 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B123" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E123">
         <v>1</v>
@@ -2758,50 +2765,47 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B124" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E124">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B125" t="s">
-        <v>173</v>
-      </c>
-      <c r="D125" s="1"/>
+        <v>171</v>
+      </c>
       <c r="E125">
         <v>1.5</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B126" t="s">
-        <v>97</v>
-      </c>
-      <c r="C126" t="s">
-        <v>182</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="D126" s="1"/>
       <c r="E126">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B127" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C127" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E127">
         <v>2</v>
@@ -2809,21 +2813,24 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>65</v>
+        <v>149</v>
       </c>
       <c r="B128" t="s">
-        <v>66</v>
+        <v>96</v>
+      </c>
+      <c r="C128" t="s">
+        <v>182</v>
       </c>
       <c r="E128">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
+        <v>64</v>
+      </c>
+      <c r="B129" t="s">
         <v>65</v>
-      </c>
-      <c r="B129" t="s">
-        <v>67</v>
       </c>
       <c r="E129">
         <v>1</v>
@@ -2831,10 +2838,10 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B130" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E130">
         <v>1</v>
@@ -2842,10 +2849,10 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B131" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E131">
         <v>1</v>
@@ -2853,43 +2860,43 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B132" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E132">
-        <v>2.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B133" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E133">
-        <v>2</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B134" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E134">
-        <v>1.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B135" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E135">
         <v>1.5</v>
@@ -2897,10 +2904,10 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B136" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E136">
         <v>1.5</v>
@@ -2908,32 +2915,32 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B137" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E137">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B138" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E138">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B139" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E139">
         <v>1</v>
@@ -2941,32 +2948,32 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B140" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E140">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B141" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E141">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B142" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E142">
         <v>1</v>
@@ -2974,32 +2981,32 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B143" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E143">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B144" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E144">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B145" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E145">
         <v>1</v>
@@ -3007,10 +3014,10 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B146" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E146">
         <v>1</v>
@@ -3018,10 +3025,10 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B147" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E147">
         <v>1</v>
@@ -3029,10 +3036,10 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B148" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E148">
         <v>1</v>
@@ -3040,10 +3047,10 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B149" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E149">
         <v>1</v>
@@ -3051,10 +3058,10 @@
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B150" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E150">
         <v>1</v>
@@ -3062,32 +3069,32 @@
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B151" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E151">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B152" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E152">
-        <v>1.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B153" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E153">
         <v>1.5</v>
@@ -3095,10 +3102,10 @@
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B154" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E154">
         <v>1.5</v>
@@ -3106,57 +3113,54 @@
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B155" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E155">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B156" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E156">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B157" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E157">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B158" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E158">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B159" t="s">
-        <v>97</v>
-      </c>
-      <c r="C159" t="s">
-        <v>66</v>
+        <v>95</v>
       </c>
       <c r="E159">
         <v>1</v>
@@ -3164,99 +3168,98 @@
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
+        <v>64</v>
+      </c>
+      <c r="B160" t="s">
+        <v>96</v>
+      </c>
+      <c r="C160" t="s">
         <v>65</v>
       </c>
-      <c r="B160" t="s">
-        <v>97</v>
-      </c>
-      <c r="C160" t="s">
-        <v>98</v>
-      </c>
       <c r="E160">
-        <v>3.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B161" t="s">
+        <v>96</v>
+      </c>
+      <c r="C161" t="s">
         <v>97</v>
       </c>
-      <c r="C161" t="s">
-        <v>99</v>
-      </c>
       <c r="E161">
-        <v>3.2</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B162" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C162" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E162">
-        <v>0.7</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B163" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C163" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E163">
-        <v>1.5</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B164" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C164" t="s">
-        <v>102</v>
-      </c>
-      <c r="D164" s="1"/>
+        <v>100</v>
+      </c>
       <c r="E164">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B165" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C165" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D165" s="1"/>
       <c r="E165">
-        <v>0.7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B166" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C166" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D166" s="1"/>
       <c r="E166">
@@ -3265,28 +3268,28 @@
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B167" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C167" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D167" s="1"/>
       <c r="E167">
-        <v>2</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B168" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C168" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D168" s="1"/>
       <c r="E168">
@@ -3295,13 +3298,13 @@
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B169" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C169" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D169" s="1"/>
       <c r="E169">
@@ -3310,13 +3313,13 @@
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B170" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C170" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D170" s="1"/>
       <c r="E170">
@@ -3325,13 +3328,13 @@
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B171" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C171" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D171" s="1"/>
       <c r="E171">
@@ -3340,79 +3343,80 @@
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B172" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C172" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D172" s="1"/>
       <c r="E172">
-        <v>1.2</v>
+        <v>2</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B173" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C173" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D173" s="1"/>
       <c r="E173">
-        <v>2</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>65</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="B174" t="s">
+        <v>96</v>
+      </c>
+      <c r="C174" t="s">
+        <v>110</v>
+      </c>
+      <c r="D174" s="1"/>
       <c r="E174">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>65</v>
-      </c>
-      <c r="B175" t="s">
-        <v>137</v>
-      </c>
-      <c r="C175" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="E175">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B176" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C176" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="E176">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B177" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C177" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E177">
         <v>1</v>
@@ -3420,27 +3424,27 @@
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B178" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C178" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="E178">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B179" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C179" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E179">
         <v>1.5</v>
@@ -3448,110 +3452,113 @@
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B180" t="s">
-        <v>138</v>
+        <v>136</v>
+      </c>
+      <c r="C180" t="s">
+        <v>89</v>
       </c>
       <c r="E180">
-        <v>3</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B181" t="s">
         <v>137</v>
       </c>
       <c r="E181">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B182" t="s">
-        <v>137</v>
-      </c>
-      <c r="C182" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E182">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B183" t="s">
-        <v>139</v>
+        <v>136</v>
+      </c>
+      <c r="C183" t="s">
+        <v>137</v>
       </c>
       <c r="E183">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B184" t="s">
-        <v>137</v>
-      </c>
-      <c r="C184" t="s">
-        <v>84</v>
+        <v>138</v>
       </c>
       <c r="E184">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B185" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C185" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="E185">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B186" t="s">
-        <v>140</v>
+        <v>136</v>
+      </c>
+      <c r="C186" t="s">
+        <v>73</v>
       </c>
       <c r="E186">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B187" t="s">
-        <v>137</v>
-      </c>
-      <c r="C187" t="s">
-        <v>67</v>
+        <v>139</v>
       </c>
       <c r="E187">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B188" t="s">
-        <v>141</v>
+        <v>136</v>
+      </c>
+      <c r="C188" t="s">
+        <v>66</v>
       </c>
       <c r="E188">
         <v>1</v>
@@ -3559,68 +3566,64 @@
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B189" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="E189">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B190" t="s">
-        <v>97</v>
-      </c>
-      <c r="C190" t="s">
-        <v>174</v>
+        <v>151</v>
       </c>
       <c r="E190">
         <v>2</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A191" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B191" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C191" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="D191" s="4"/>
+      <c r="A191" t="s">
+        <v>64</v>
+      </c>
+      <c r="B191" t="s">
+        <v>96</v>
+      </c>
+      <c r="C191" t="s">
+        <v>173</v>
+      </c>
       <c r="E191">
-        <v>0.7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A192" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>176</v>
+        <v>96</v>
       </c>
       <c r="C192" s="3" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D192" s="4"/>
       <c r="E192">
-        <v>2</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A193" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>97</v>
+        <v>175</v>
       </c>
       <c r="C193" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D193" s="4"/>
       <c r="E193">
@@ -3629,42 +3632,42 @@
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A194" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C194" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D194" s="4"/>
       <c r="E194">
-        <v>1.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A195" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C195" s="3"/>
+        <v>96</v>
+      </c>
+      <c r="C195" s="3" t="s">
+        <v>178</v>
+      </c>
       <c r="D195" s="4"/>
       <c r="E195">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A196" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C196" s="3" t="s">
-        <v>180</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="C196" s="3"/>
       <c r="D196" s="4"/>
       <c r="E196">
         <v>2</v>
@@ -3672,17 +3675,46 @@
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A197" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C197" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D197" s="4"/>
       <c r="E197">
         <v>2</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A198" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B198" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C198" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="D198" s="4"/>
+      <c r="E198">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A199" t="s">
+        <v>64</v>
+      </c>
+      <c r="B199" t="s">
+        <v>189</v>
+      </c>
+      <c r="C199" t="s">
+        <v>185</v>
+      </c>
+      <c r="E199">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mappings for new sephora categories done
</commit_message>
<xml_diff>
--- a/product_scraper/product_scraper/reference_data/profit_margin_mapping.xlsx
+++ b/product_scraper/product_scraper/reference_data/profit_margin_mapping.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/CodeForLyf/qarece-web-crawler/product_scraper/product_scraper/reference_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sujilmaharjan/Desktop/qarece-web-crawler/product_scraper/product_scraper/reference_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F62D9A01-9ABB-D14F-BBF3-492B82139A41}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{579B68AF-12A5-2940-9EDB-044C32216868}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{DABBC373-DD1C-BE4F-B648-BD9F3D1B3B72}"/>
   </bookViews>
   <sheets>
     <sheet name="Average" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="195">
   <si>
     <t>Handbags</t>
   </si>
@@ -601,6 +601,21 @@
   </si>
   <si>
     <t>Fragrances &amp; Perfumes</t>
+  </si>
+  <si>
+    <t>Hair</t>
+  </si>
+  <si>
+    <t>Hair Dryers</t>
+  </si>
+  <si>
+    <t>Candles &amp; Home Scents</t>
+  </si>
+  <si>
+    <t>Bath &amp; Body</t>
+  </si>
+  <si>
+    <t>Hair Oil</t>
   </si>
 </sst>
 </file>
@@ -708,9 +723,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{013CB231-6A17-0C41-B34E-8545193EC78F}" name="Table3" displayName="Table3" ref="A1:E200" totalsRowShown="0">
-  <autoFilter ref="A1:E200" xr:uid="{80DC04BB-911F-774F-8154-5B368973EF57}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E198">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{013CB231-6A17-0C41-B34E-8545193EC78F}" name="Table3" displayName="Table3" ref="A1:E211" totalsRowShown="0">
+  <autoFilter ref="A1:E211" xr:uid="{80DC04BB-911F-774F-8154-5B368973EF57}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E211">
     <sortCondition ref="A1:A1048571"/>
   </sortState>
   <tableColumns count="5">
@@ -1021,10 +1036,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{674E1AF3-8D38-BC46-B033-52B0C55ED4E6}">
-  <dimension ref="A1:E199"/>
+  <dimension ref="A1:E211"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2165,77 +2180,97 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>152</v>
+        <v>21</v>
       </c>
       <c r="B70" t="s">
-        <v>153</v>
+        <v>190</v>
+      </c>
+      <c r="C70" t="s">
+        <v>191</v>
       </c>
       <c r="E70">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B71" t="s">
-        <v>12</v>
+        <v>56</v>
+      </c>
+      <c r="C71" t="s">
+        <v>33</v>
+      </c>
+      <c r="D71" t="s">
+        <v>114</v>
       </c>
       <c r="E71">
-        <v>3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B72" t="s">
-        <v>1</v>
-      </c>
-      <c r="D72" s="1"/>
+        <v>190</v>
+      </c>
+      <c r="C72" t="s">
+        <v>185</v>
+      </c>
       <c r="E72">
         <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B73" t="s">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="E73">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B74" t="s">
-        <v>13</v>
+        <v>149</v>
+      </c>
+      <c r="C74" t="s">
+        <v>185</v>
       </c>
       <c r="E74">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B75" t="s">
-        <v>14</v>
+        <v>189</v>
+      </c>
+      <c r="C75" t="s">
+        <v>185</v>
       </c>
       <c r="E75">
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B76" t="s">
-        <v>3</v>
+        <v>189</v>
+      </c>
+      <c r="C76" t="s">
+        <v>192</v>
       </c>
       <c r="E76">
         <v>1.5</v>
@@ -2243,33 +2278,35 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B77" t="s">
-        <v>15</v>
+        <v>193</v>
+      </c>
+      <c r="C77" t="s">
+        <v>185</v>
       </c>
       <c r="E77">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B78" t="s">
-        <v>16</v>
-      </c>
-      <c r="D78" s="1"/>
+        <v>189</v>
+      </c>
       <c r="E78">
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B79" t="s">
-        <v>17</v>
+        <v>190</v>
       </c>
       <c r="E79">
         <v>1.5</v>
@@ -2277,26 +2314,27 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B80" t="s">
-        <v>4</v>
-      </c>
-      <c r="D80" s="1"/>
+        <v>190</v>
+      </c>
+      <c r="C80" t="s">
+        <v>194</v>
+      </c>
       <c r="E80">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>0</v>
+        <v>152</v>
       </c>
       <c r="B81" t="s">
-        <v>5</v>
-      </c>
-      <c r="D81" s="1"/>
+        <v>153</v>
+      </c>
       <c r="E81">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
@@ -2304,11 +2342,10 @@
         <v>0</v>
       </c>
       <c r="B82" t="s">
-        <v>6</v>
-      </c>
-      <c r="D82" s="1"/>
+        <v>12</v>
+      </c>
       <c r="E82">
-        <v>2.7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
@@ -2316,10 +2353,11 @@
         <v>0</v>
       </c>
       <c r="B83" t="s">
-        <v>7</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D83" s="1"/>
       <c r="E83">
-        <v>2.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
@@ -2327,10 +2365,10 @@
         <v>0</v>
       </c>
       <c r="B84" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="E84">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
@@ -2338,10 +2376,10 @@
         <v>0</v>
       </c>
       <c r="B85" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E85">
-        <v>0.8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
@@ -2349,10 +2387,10 @@
         <v>0</v>
       </c>
       <c r="B86" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E86">
-        <v>0.5</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
@@ -2360,10 +2398,10 @@
         <v>0</v>
       </c>
       <c r="B87" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E87">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
@@ -2371,10 +2409,10 @@
         <v>0</v>
       </c>
       <c r="B88" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E88">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
@@ -2382,10 +2420,11 @@
         <v>0</v>
       </c>
       <c r="B89" t="s">
-        <v>8</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="D89" s="1"/>
       <c r="E89">
-        <v>0.8</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
@@ -2393,18 +2432,22 @@
         <v>0</v>
       </c>
       <c r="B90" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E90">
-        <v>0.2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>0</v>
       </c>
+      <c r="B91" t="s">
+        <v>4</v>
+      </c>
+      <c r="D91" s="1"/>
       <c r="E91">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
@@ -2412,13 +2455,11 @@
         <v>0</v>
       </c>
       <c r="B92" t="s">
-        <v>141</v>
-      </c>
-      <c r="C92" t="s">
-        <v>142</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D92" s="1"/>
       <c r="E92">
-        <v>1.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
@@ -2426,13 +2467,11 @@
         <v>0</v>
       </c>
       <c r="B93" t="s">
-        <v>141</v>
-      </c>
-      <c r="C93" t="s">
-        <v>145</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D93" s="1"/>
       <c r="E93">
-        <v>2</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
@@ -2440,13 +2479,10 @@
         <v>0</v>
       </c>
       <c r="B94" t="s">
-        <v>146</v>
-      </c>
-      <c r="C94" t="s">
-        <v>147</v>
+        <v>7</v>
       </c>
       <c r="E94">
-        <v>2</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
@@ -2454,7 +2490,7 @@
         <v>0</v>
       </c>
       <c r="B95" t="s">
-        <v>148</v>
+        <v>18</v>
       </c>
       <c r="E95">
         <v>2</v>
@@ -2462,142 +2498,148 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>143</v>
+        <v>0</v>
       </c>
       <c r="B96" t="s">
-        <v>144</v>
+        <v>19</v>
       </c>
       <c r="E96">
-        <v>2</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>143</v>
+        <v>0</v>
+      </c>
+      <c r="B97" t="s">
+        <v>10</v>
       </c>
       <c r="E97">
-        <v>2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>149</v>
+        <v>0</v>
       </c>
       <c r="B98" t="s">
-        <v>150</v>
+        <v>9</v>
       </c>
       <c r="E98">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>149</v>
+        <v>0</v>
       </c>
       <c r="B99" t="s">
-        <v>154</v>
+        <v>11</v>
       </c>
       <c r="E99">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>149</v>
+        <v>0</v>
       </c>
       <c r="B100" t="s">
-        <v>89</v>
+        <v>8</v>
       </c>
       <c r="E100">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>149</v>
+        <v>0</v>
       </c>
       <c r="B101" t="s">
-        <v>155</v>
+        <v>20</v>
       </c>
       <c r="E101">
-        <v>1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>149</v>
-      </c>
-      <c r="B102" t="s">
-        <v>156</v>
+        <v>0</v>
       </c>
       <c r="E102">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>149</v>
+        <v>0</v>
       </c>
       <c r="B103" t="s">
-        <v>79</v>
+        <v>141</v>
+      </c>
+      <c r="C103" t="s">
+        <v>142</v>
       </c>
       <c r="E103">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>149</v>
+        <v>0</v>
       </c>
       <c r="B104" t="s">
-        <v>157</v>
+        <v>141</v>
+      </c>
+      <c r="C104" t="s">
+        <v>145</v>
       </c>
       <c r="E104">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>149</v>
+        <v>0</v>
       </c>
       <c r="B105" t="s">
-        <v>158</v>
+        <v>146</v>
+      </c>
+      <c r="C105" t="s">
+        <v>147</v>
       </c>
       <c r="E105">
-        <v>1.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>149</v>
+        <v>0</v>
       </c>
       <c r="B106" t="s">
-        <v>86</v>
+        <v>148</v>
       </c>
       <c r="E106">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B107" t="s">
-        <v>73</v>
+        <v>144</v>
       </c>
       <c r="E107">
-        <v>1.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>149</v>
-      </c>
-      <c r="B108" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
       <c r="E108">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
@@ -2605,7 +2647,7 @@
         <v>149</v>
       </c>
       <c r="B109" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="E109">
         <v>1.5</v>
@@ -2616,10 +2658,10 @@
         <v>149</v>
       </c>
       <c r="B110" t="s">
-        <v>183</v>
+        <v>154</v>
       </c>
       <c r="E110">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
@@ -2627,10 +2669,10 @@
         <v>149</v>
       </c>
       <c r="B111" t="s">
-        <v>161</v>
+        <v>89</v>
       </c>
       <c r="E111">
-        <v>3</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
@@ -2638,7 +2680,7 @@
         <v>149</v>
       </c>
       <c r="B112" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="E112">
         <v>1</v>
@@ -2649,7 +2691,7 @@
         <v>149</v>
       </c>
       <c r="B113" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="E113">
         <v>1</v>
@@ -2660,10 +2702,10 @@
         <v>149</v>
       </c>
       <c r="B114" t="s">
-        <v>164</v>
+        <v>79</v>
       </c>
       <c r="E114">
-        <v>3.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
@@ -2671,18 +2713,21 @@
         <v>149</v>
       </c>
       <c r="B115" t="s">
-        <v>184</v>
+        <v>157</v>
       </c>
       <c r="E115">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>149</v>
       </c>
+      <c r="B116" t="s">
+        <v>158</v>
+      </c>
       <c r="E116">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
@@ -2690,7 +2735,7 @@
         <v>149</v>
       </c>
       <c r="B117" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="E117">
         <v>1</v>
@@ -2701,10 +2746,10 @@
         <v>149</v>
       </c>
       <c r="B118" t="s">
-        <v>165</v>
+        <v>73</v>
       </c>
       <c r="E118">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
@@ -2712,7 +2757,7 @@
         <v>149</v>
       </c>
       <c r="B119" t="s">
-        <v>83</v>
+        <v>159</v>
       </c>
       <c r="D119" s="2"/>
       <c r="E119">
@@ -2724,10 +2769,10 @@
         <v>149</v>
       </c>
       <c r="B120" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="E120">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
@@ -2735,7 +2780,7 @@
         <v>149</v>
       </c>
       <c r="B121" t="s">
-        <v>167</v>
+        <v>183</v>
       </c>
       <c r="E121">
         <v>1</v>
@@ -2746,10 +2791,10 @@
         <v>149</v>
       </c>
       <c r="B122" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="E122">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
@@ -2757,7 +2802,7 @@
         <v>149</v>
       </c>
       <c r="B123" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="E123">
         <v>1</v>
@@ -2768,7 +2813,7 @@
         <v>149</v>
       </c>
       <c r="B124" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="E124">
         <v>1</v>
@@ -2779,10 +2824,10 @@
         <v>149</v>
       </c>
       <c r="B125" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="E125">
-        <v>1.5</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
@@ -2790,9 +2835,8 @@
         <v>149</v>
       </c>
       <c r="B126" t="s">
-        <v>172</v>
-      </c>
-      <c r="D126" s="1"/>
+        <v>184</v>
+      </c>
       <c r="E126">
         <v>1.5</v>
       </c>
@@ -2801,12 +2845,6 @@
       <c r="A127" t="s">
         <v>149</v>
       </c>
-      <c r="B127" t="s">
-        <v>96</v>
-      </c>
-      <c r="C127" t="s">
-        <v>181</v>
-      </c>
       <c r="E127">
         <v>2</v>
       </c>
@@ -2816,21 +2854,18 @@
         <v>149</v>
       </c>
       <c r="B128" t="s">
-        <v>96</v>
-      </c>
-      <c r="C128" t="s">
-        <v>182</v>
+        <v>95</v>
       </c>
       <c r="E128">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>64</v>
+        <v>149</v>
       </c>
       <c r="B129" t="s">
-        <v>65</v>
+        <v>165</v>
       </c>
       <c r="E129">
         <v>1</v>
@@ -2838,21 +2873,22 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>64</v>
+        <v>149</v>
       </c>
       <c r="B130" t="s">
-        <v>66</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="D130" s="1"/>
       <c r="E130">
         <v>1</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>64</v>
+        <v>149</v>
       </c>
       <c r="B131" t="s">
-        <v>67</v>
+        <v>166</v>
       </c>
       <c r="E131">
         <v>1</v>
@@ -2860,10 +2896,10 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>64</v>
+        <v>149</v>
       </c>
       <c r="B132" t="s">
-        <v>68</v>
+        <v>167</v>
       </c>
       <c r="E132">
         <v>1</v>
@@ -2871,43 +2907,43 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>64</v>
+        <v>149</v>
       </c>
       <c r="B133" t="s">
-        <v>69</v>
+        <v>168</v>
       </c>
       <c r="E133">
-        <v>2.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>64</v>
+        <v>149</v>
       </c>
       <c r="B134" t="s">
-        <v>70</v>
+        <v>169</v>
       </c>
       <c r="E134">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>64</v>
+        <v>149</v>
       </c>
       <c r="B135" t="s">
-        <v>71</v>
+        <v>170</v>
       </c>
       <c r="E135">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>64</v>
+        <v>149</v>
       </c>
       <c r="B136" t="s">
-        <v>72</v>
+        <v>171</v>
       </c>
       <c r="E136">
         <v>1.5</v>
@@ -2915,21 +2951,25 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>64</v>
+        <v>149</v>
       </c>
       <c r="B137" t="s">
-        <v>73</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="D137" s="1"/>
       <c r="E137">
         <v>1.5</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>64</v>
+        <v>149</v>
       </c>
       <c r="B138" t="s">
-        <v>74</v>
+        <v>96</v>
+      </c>
+      <c r="C138" t="s">
+        <v>181</v>
       </c>
       <c r="E138">
         <v>2</v>
@@ -2937,13 +2977,16 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>64</v>
+        <v>149</v>
       </c>
       <c r="B139" t="s">
-        <v>75</v>
+        <v>96</v>
+      </c>
+      <c r="C139" t="s">
+        <v>182</v>
       </c>
       <c r="E139">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
@@ -2951,7 +2994,7 @@
         <v>64</v>
       </c>
       <c r="B140" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="E140">
         <v>1</v>
@@ -2962,10 +3005,10 @@
         <v>64</v>
       </c>
       <c r="B141" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="E141">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
@@ -2973,7 +3016,7 @@
         <v>64</v>
       </c>
       <c r="B142" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="E142">
         <v>1</v>
@@ -2984,7 +3027,7 @@
         <v>64</v>
       </c>
       <c r="B143" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="E143">
         <v>1</v>
@@ -2995,10 +3038,10 @@
         <v>64</v>
       </c>
       <c r="B144" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="E144">
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
@@ -3006,10 +3049,10 @@
         <v>64</v>
       </c>
       <c r="B145" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="E145">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
@@ -3017,10 +3060,10 @@
         <v>64</v>
       </c>
       <c r="B146" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="E146">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
@@ -3028,10 +3071,10 @@
         <v>64</v>
       </c>
       <c r="B147" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="E147">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.2">
@@ -3039,10 +3082,10 @@
         <v>64</v>
       </c>
       <c r="B148" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="E148">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.2">
@@ -3050,10 +3093,10 @@
         <v>64</v>
       </c>
       <c r="B149" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="E149">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.2">
@@ -3061,7 +3104,7 @@
         <v>64</v>
       </c>
       <c r="B150" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="E150">
         <v>1</v>
@@ -3072,7 +3115,7 @@
         <v>64</v>
       </c>
       <c r="B151" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="E151">
         <v>1</v>
@@ -3083,10 +3126,10 @@
         <v>64</v>
       </c>
       <c r="B152" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="E152">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.2">
@@ -3094,10 +3137,10 @@
         <v>64</v>
       </c>
       <c r="B153" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="E153">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.2">
@@ -3105,10 +3148,10 @@
         <v>64</v>
       </c>
       <c r="B154" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="E154">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.2">
@@ -3116,7 +3159,7 @@
         <v>64</v>
       </c>
       <c r="B155" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="E155">
         <v>1.5</v>
@@ -3127,7 +3170,7 @@
         <v>64</v>
       </c>
       <c r="B156" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="E156">
         <v>1</v>
@@ -3138,10 +3181,10 @@
         <v>64</v>
       </c>
       <c r="B157" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="E157">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.2">
@@ -3149,10 +3192,10 @@
         <v>64</v>
       </c>
       <c r="B158" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="E158">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.2">
@@ -3160,7 +3203,7 @@
         <v>64</v>
       </c>
       <c r="B159" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="E159">
         <v>1</v>
@@ -3171,10 +3214,7 @@
         <v>64</v>
       </c>
       <c r="B160" t="s">
-        <v>96</v>
-      </c>
-      <c r="C160" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="E160">
         <v>1</v>
@@ -3185,13 +3225,10 @@
         <v>64</v>
       </c>
       <c r="B161" t="s">
-        <v>96</v>
-      </c>
-      <c r="C161" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="E161">
-        <v>3.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.2">
@@ -3199,13 +3236,10 @@
         <v>64</v>
       </c>
       <c r="B162" t="s">
-        <v>96</v>
-      </c>
-      <c r="C162" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="E162">
-        <v>3.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.2">
@@ -3213,13 +3247,10 @@
         <v>64</v>
       </c>
       <c r="B163" t="s">
-        <v>96</v>
-      </c>
-      <c r="C163" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="E163">
-        <v>0.7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.2">
@@ -3227,10 +3258,7 @@
         <v>64</v>
       </c>
       <c r="B164" t="s">
-        <v>96</v>
-      </c>
-      <c r="C164" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="E164">
         <v>1.5</v>
@@ -3241,14 +3269,10 @@
         <v>64</v>
       </c>
       <c r="B165" t="s">
-        <v>96</v>
-      </c>
-      <c r="C165" t="s">
-        <v>101</v>
-      </c>
-      <c r="D165" s="1"/>
+        <v>90</v>
+      </c>
       <c r="E165">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.2">
@@ -3256,14 +3280,10 @@
         <v>64</v>
       </c>
       <c r="B166" t="s">
-        <v>96</v>
-      </c>
-      <c r="C166" t="s">
-        <v>102</v>
-      </c>
-      <c r="D166" s="1"/>
+        <v>91</v>
+      </c>
       <c r="E166">
-        <v>0.7</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.2">
@@ -3271,14 +3291,10 @@
         <v>64</v>
       </c>
       <c r="B167" t="s">
-        <v>96</v>
-      </c>
-      <c r="C167" t="s">
-        <v>103</v>
-      </c>
-      <c r="D167" s="1"/>
+        <v>92</v>
+      </c>
       <c r="E167">
-        <v>0.7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.2">
@@ -3286,14 +3302,10 @@
         <v>64</v>
       </c>
       <c r="B168" t="s">
-        <v>96</v>
-      </c>
-      <c r="C168" t="s">
-        <v>104</v>
-      </c>
-      <c r="D168" s="1"/>
+        <v>93</v>
+      </c>
       <c r="E168">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.2">
@@ -3301,12 +3313,8 @@
         <v>64</v>
       </c>
       <c r="B169" t="s">
-        <v>96</v>
-      </c>
-      <c r="C169" t="s">
-        <v>105</v>
-      </c>
-      <c r="D169" s="1"/>
+        <v>94</v>
+      </c>
       <c r="E169">
         <v>2</v>
       </c>
@@ -3316,14 +3324,10 @@
         <v>64</v>
       </c>
       <c r="B170" t="s">
-        <v>96</v>
-      </c>
-      <c r="C170" t="s">
-        <v>106</v>
-      </c>
-      <c r="D170" s="1"/>
+        <v>95</v>
+      </c>
       <c r="E170">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.2">
@@ -3334,11 +3338,10 @@
         <v>96</v>
       </c>
       <c r="C171" t="s">
-        <v>107</v>
-      </c>
-      <c r="D171" s="1"/>
+        <v>65</v>
+      </c>
       <c r="E171">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.2">
@@ -3349,11 +3352,10 @@
         <v>96</v>
       </c>
       <c r="C172" t="s">
-        <v>108</v>
-      </c>
-      <c r="D172" s="1"/>
+        <v>97</v>
+      </c>
       <c r="E172">
-        <v>2</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.2">
@@ -3364,11 +3366,10 @@
         <v>96</v>
       </c>
       <c r="C173" t="s">
-        <v>109</v>
-      </c>
-      <c r="D173" s="1"/>
+        <v>98</v>
+      </c>
       <c r="E173">
-        <v>1.2</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
@@ -3379,19 +3380,24 @@
         <v>96</v>
       </c>
       <c r="C174" t="s">
-        <v>110</v>
-      </c>
-      <c r="D174" s="1"/>
+        <v>99</v>
+      </c>
       <c r="E174">
-        <v>2</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>64</v>
       </c>
+      <c r="B175" t="s">
+        <v>96</v>
+      </c>
+      <c r="C175" t="s">
+        <v>100</v>
+      </c>
       <c r="E175">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.2">
@@ -3399,11 +3405,12 @@
         <v>64</v>
       </c>
       <c r="B176" t="s">
-        <v>136</v>
+        <v>96</v>
       </c>
       <c r="C176" t="s">
-        <v>70</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="D176" s="1"/>
       <c r="E176">
         <v>2</v>
       </c>
@@ -3413,13 +3420,14 @@
         <v>64</v>
       </c>
       <c r="B177" t="s">
-        <v>136</v>
+        <v>96</v>
       </c>
       <c r="C177" t="s">
-        <v>79</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="D177" s="1"/>
       <c r="E177">
-        <v>1</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.2">
@@ -3427,13 +3435,14 @@
         <v>64</v>
       </c>
       <c r="B178" t="s">
-        <v>136</v>
+        <v>96</v>
       </c>
       <c r="C178" t="s">
-        <v>84</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="D178" s="1"/>
       <c r="E178">
-        <v>1</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.2">
@@ -3441,13 +3450,14 @@
         <v>64</v>
       </c>
       <c r="B179" t="s">
-        <v>136</v>
+        <v>96</v>
       </c>
       <c r="C179" t="s">
-        <v>93</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="D179" s="1"/>
       <c r="E179">
-        <v>1.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.2">
@@ -3455,13 +3465,14 @@
         <v>64</v>
       </c>
       <c r="B180" t="s">
-        <v>136</v>
+        <v>96</v>
       </c>
       <c r="C180" t="s">
-        <v>89</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="D180" s="1"/>
       <c r="E180">
-        <v>1.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.2">
@@ -3469,10 +3480,14 @@
         <v>64</v>
       </c>
       <c r="B181" t="s">
-        <v>137</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="C181" t="s">
+        <v>106</v>
+      </c>
+      <c r="D181" s="1"/>
       <c r="E181">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.2">
@@ -3480,8 +3495,12 @@
         <v>64</v>
       </c>
       <c r="B182" t="s">
-        <v>136</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="C182" t="s">
+        <v>107</v>
+      </c>
+      <c r="D182" s="1"/>
       <c r="E182">
         <v>2</v>
       </c>
@@ -3491,13 +3510,14 @@
         <v>64</v>
       </c>
       <c r="B183" t="s">
-        <v>136</v>
+        <v>96</v>
       </c>
       <c r="C183" t="s">
-        <v>137</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="D183" s="1"/>
       <c r="E183">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.2">
@@ -3505,10 +3525,14 @@
         <v>64</v>
       </c>
       <c r="B184" t="s">
-        <v>138</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="C184" t="s">
+        <v>109</v>
+      </c>
+      <c r="D184" s="1"/>
       <c r="E184">
-        <v>2</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.2">
@@ -3516,27 +3540,22 @@
         <v>64</v>
       </c>
       <c r="B185" t="s">
-        <v>136</v>
+        <v>96</v>
       </c>
       <c r="C185" t="s">
-        <v>83</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="D185" s="1"/>
       <c r="E185">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>64</v>
       </c>
-      <c r="B186" t="s">
-        <v>136</v>
-      </c>
-      <c r="C186" t="s">
-        <v>73</v>
-      </c>
       <c r="E186">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.2">
@@ -3544,7 +3563,10 @@
         <v>64</v>
       </c>
       <c r="B187" t="s">
-        <v>139</v>
+        <v>136</v>
+      </c>
+      <c r="C187" t="s">
+        <v>70</v>
       </c>
       <c r="E187">
         <v>2</v>
@@ -3558,7 +3580,7 @@
         <v>136</v>
       </c>
       <c r="C188" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="E188">
         <v>1</v>
@@ -3569,7 +3591,10 @@
         <v>64</v>
       </c>
       <c r="B189" t="s">
-        <v>140</v>
+        <v>136</v>
+      </c>
+      <c r="C189" t="s">
+        <v>84</v>
       </c>
       <c r="E189">
         <v>1</v>
@@ -3580,10 +3605,13 @@
         <v>64</v>
       </c>
       <c r="B190" t="s">
-        <v>151</v>
+        <v>136</v>
+      </c>
+      <c r="C190" t="s">
+        <v>93</v>
       </c>
       <c r="E190">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.2">
@@ -3591,13 +3619,13 @@
         <v>64</v>
       </c>
       <c r="B191" t="s">
-        <v>96</v>
+        <v>136</v>
       </c>
       <c r="C191" t="s">
-        <v>173</v>
+        <v>89</v>
       </c>
       <c r="E191">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.2">
@@ -3605,14 +3633,12 @@
         <v>64</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C192" s="3" t="s">
-        <v>174</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="C192" s="3"/>
       <c r="D192" s="4"/>
       <c r="E192">
-        <v>0.7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.2">
@@ -3620,11 +3646,9 @@
         <v>64</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="C193" s="3" t="s">
-        <v>176</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="C193" s="3"/>
       <c r="D193" s="4"/>
       <c r="E193">
         <v>2</v>
@@ -3635,14 +3659,14 @@
         <v>64</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>96</v>
+        <v>136</v>
       </c>
       <c r="C194" s="3" t="s">
-        <v>177</v>
+        <v>137</v>
       </c>
       <c r="D194" s="4"/>
       <c r="E194">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.2">
@@ -3650,14 +3674,12 @@
         <v>64</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C195" s="3" t="s">
-        <v>178</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="C195" s="3"/>
       <c r="D195" s="4"/>
       <c r="E195">
-        <v>1.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.2">
@@ -3665,12 +3687,14 @@
         <v>64</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C196" s="3"/>
+        <v>136</v>
+      </c>
+      <c r="C196" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="D196" s="4"/>
       <c r="E196">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.2">
@@ -3678,14 +3702,14 @@
         <v>64</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>96</v>
+        <v>136</v>
       </c>
       <c r="C197" s="3" t="s">
-        <v>179</v>
+        <v>73</v>
       </c>
       <c r="D197" s="4"/>
       <c r="E197">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.2">
@@ -3693,11 +3717,9 @@
         <v>64</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C198" s="3" t="s">
-        <v>180</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="C198" s="3"/>
       <c r="D198" s="4"/>
       <c r="E198">
         <v>2</v>
@@ -3708,12 +3730,176 @@
         <v>64</v>
       </c>
       <c r="B199" t="s">
+        <v>136</v>
+      </c>
+      <c r="C199" t="s">
+        <v>66</v>
+      </c>
+      <c r="E199">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A200" t="s">
+        <v>64</v>
+      </c>
+      <c r="B200" t="s">
+        <v>140</v>
+      </c>
+      <c r="E200">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A201" t="s">
+        <v>64</v>
+      </c>
+      <c r="B201" t="s">
+        <v>151</v>
+      </c>
+      <c r="E201">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A202" t="s">
+        <v>64</v>
+      </c>
+      <c r="B202" t="s">
+        <v>96</v>
+      </c>
+      <c r="C202" t="s">
+        <v>173</v>
+      </c>
+      <c r="E202">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A203" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C203" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D203" s="1"/>
+      <c r="E203">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A204" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B204" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C204" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D204" s="1"/>
+      <c r="E204">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A205" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C205" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D205" s="1"/>
+      <c r="E205">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A206" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B206" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C206" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D206" s="1"/>
+      <c r="E206">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A207" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B207" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C207" s="1"/>
+      <c r="D207" s="1"/>
+      <c r="E207">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A208" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B208" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C208" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D208" s="1"/>
+      <c r="E208">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A209" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B209" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C209" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D209" s="1"/>
+      <c r="E209">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A210" t="s">
+        <v>64</v>
+      </c>
+      <c r="B210" t="s">
         <v>189</v>
       </c>
-      <c r="C199" t="s">
+      <c r="C210" t="s">
         <v>185</v>
       </c>
-      <c r="E199">
+      <c r="E210">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A211" t="s">
+        <v>64</v>
+      </c>
+      <c r="B211" t="s">
+        <v>189</v>
+      </c>
+      <c r="E211">
         <v>1</v>
       </c>
     </row>

</xml_diff>